<commit_message>
nem írható versenyID, gombre generálódó versenyID
</commit_message>
<xml_diff>
--- a/database/versenyekDB.xlsx
+++ b/database/versenyekDB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,56 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>VID_00002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>VID_00003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>VID_00004</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>VID_00005</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>VID_00006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
frissen felvett mentés eredményekbe emelése
</commit_message>
<xml_diff>
--- a/database/versenyekDB.xlsx
+++ b/database/versenyekDB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,6 +527,16 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>VID_00007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>